<commit_message>
reuploaded reference CM file
</commit_message>
<xml_diff>
--- a/Ref_known_CMs.xlsx
+++ b/Ref_known_CMs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/viktoriabrunner/Documents/Studium/PhD/Project1_rev/repository/tb-rnap-compensation/reference/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/viktoriabrunner/Documents/Studium/PhD/Project1_rev/repository/tb-rnap-compensation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BC73EA3-D792-4440-A97B-7E9EBBF5D859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DAA8C6B-1DC6-7C47-B6AE-614CD9972735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16700" yWindow="500" windowWidth="11720" windowHeight="16520" firstSheet="1" activeTab="2" xr2:uid="{011A8AAB-9AFE-8A49-A3D3-8E76BD9F0AAE}"/>
+    <workbookView xWindow="16700" yWindow="500" windowWidth="11720" windowHeight="16520" xr2:uid="{011A8AAB-9AFE-8A49-A3D3-8E76BD9F0AAE}"/>
   </bookViews>
   <sheets>
     <sheet name="described_CMs_total" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="125">
   <si>
     <t>Comas_2012</t>
   </si>
@@ -409,6 +409,9 @@
   </si>
   <si>
     <t>mutation</t>
+  </si>
+  <si>
+    <t>low probability</t>
   </si>
 </sst>
 </file>
@@ -775,10 +778,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5F31778-9697-1741-A4E9-D8CEF94BCD43}">
-  <dimension ref="A1:G97"/>
+  <dimension ref="A1:G98"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="B98" sqref="B98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3055,6 +3058,11 @@
       </c>
       <c r="E97" s="3" t="s">
         <v>83</v>
+      </c>
+    </row>
+    <row r="98" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B98" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -5354,8 +5362,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A456F73-CE23-4C41-8598-F78254EEFB29}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>